<commit_message>
changed categories color and trying to figure out how to add labels to the bubbles
</commit_message>
<xml_diff>
--- a/data/AllMoviesSummary.xlsx
+++ b/data/AllMoviesSummary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="13880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12760" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>movie</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Rogue One</t>
   </si>
   <si>
-    <t>total_female_lines</t>
-  </si>
-  <si>
-    <t>total_lines</t>
-  </si>
-  <si>
     <t>percentage_female_line</t>
   </si>
   <si>
@@ -57,6 +51,15 @@
   </si>
   <si>
     <t>radius</t>
+  </si>
+  <si>
+    <t>Batman vs. Superman</t>
+  </si>
+  <si>
+    <t>total_female_words</t>
+  </si>
+  <si>
+    <t>total_words</t>
   </si>
 </sst>
 </file>
@@ -371,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -393,16 +396,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -433,7 +436,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>13</v>
@@ -455,6 +458,20 @@
       </c>
       <c r="H3">
         <v>16.422999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>82</v>
+      </c>
+      <c r="E4">
+        <v>1583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added all the movies to index.html
</commit_message>
<xml_diff>
--- a/data/AllMoviesSummary.xlsx
+++ b/data/AllMoviesSummary.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12760" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7760"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AllMoviesSummary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>movie</t>
   </si>
@@ -41,49 +41,370 @@
     <t>percentage female_char</t>
   </si>
   <si>
+    <t>total_female_lines</t>
+  </si>
+  <si>
+    <t>total_lines</t>
+  </si>
+  <si>
+    <t>percentage_female_line</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
     <t>Rogue One</t>
   </si>
   <si>
-    <t>percentage_female_line</t>
-  </si>
-  <si>
     <t>Civil War</t>
   </si>
   <si>
-    <t>radius</t>
-  </si>
-  <si>
-    <t>Batman vs. Superman</t>
-  </si>
-  <si>
-    <t>total_female_words</t>
-  </si>
-  <si>
-    <t>total_words</t>
+    <t>BatmanVSuperman</t>
+  </si>
+  <si>
+    <t>Deadpool</t>
+  </si>
+  <si>
+    <t>Zootopia</t>
+  </si>
+  <si>
+    <t>Fantastic Beasts</t>
+  </si>
+  <si>
+    <t>Finding Dory</t>
+  </si>
+  <si>
+    <t>Jungle book</t>
+  </si>
+  <si>
+    <t>Secret Life of Pets</t>
+  </si>
+  <si>
+    <t>Suicide Squad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
+  <fonts count="18" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -91,21 +412,213 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -128,7 +641,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -140,7 +653,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -157,9 +670,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -192,9 +705,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -374,13 +887,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -396,13 +909,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -410,7 +923,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -436,7 +949,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>13</v>
@@ -462,7 +975,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -470,8 +983,202 @@
       <c r="C4">
         <v>82</v>
       </c>
+      <c r="D4">
+        <v>24.39</v>
+      </c>
       <c r="E4">
         <v>1583</v>
+      </c>
+      <c r="F4">
+        <v>7004</v>
+      </c>
+      <c r="G4">
+        <v>22.600999999999999</v>
+      </c>
+      <c r="H4">
+        <v>22.600999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>34</v>
+      </c>
+      <c r="D5">
+        <v>29.411999999999999</v>
+      </c>
+      <c r="E5">
+        <v>771</v>
+      </c>
+      <c r="F5">
+        <v>8146</v>
+      </c>
+      <c r="G5">
+        <v>9.4649999999999999</v>
+      </c>
+      <c r="H5">
+        <v>9.4649999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>49</v>
+      </c>
+      <c r="D6">
+        <v>32.652999999999999</v>
+      </c>
+      <c r="E6">
+        <v>2068</v>
+      </c>
+      <c r="F6">
+        <v>6462</v>
+      </c>
+      <c r="G6">
+        <v>32.002000000000002</v>
+      </c>
+      <c r="H6">
+        <v>32.002000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>42</v>
+      </c>
+      <c r="E7">
+        <v>5667</v>
+      </c>
+      <c r="F7">
+        <v>10709</v>
+      </c>
+      <c r="G7">
+        <v>52.917999999999999</v>
+      </c>
+      <c r="H7">
+        <v>52.917999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <v>21.428999999999998</v>
+      </c>
+      <c r="E8">
+        <v>591</v>
+      </c>
+      <c r="F8">
+        <v>5972</v>
+      </c>
+      <c r="G8">
+        <v>9.8960000000000008</v>
+      </c>
+      <c r="H8">
+        <v>9.8960000000000008</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>48</v>
+      </c>
+      <c r="D9">
+        <v>27.082999999999998</v>
+      </c>
+      <c r="E9">
+        <v>1178</v>
+      </c>
+      <c r="F9">
+        <v>6177</v>
+      </c>
+      <c r="G9">
+        <v>19.071000000000002</v>
+      </c>
+      <c r="H9">
+        <v>19.071000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>65</v>
+      </c>
+      <c r="D10">
+        <v>21.538</v>
+      </c>
+      <c r="E10">
+        <v>2427</v>
+      </c>
+      <c r="F10">
+        <v>7561</v>
+      </c>
+      <c r="G10">
+        <v>32.098999999999997</v>
+      </c>
+      <c r="H10">
+        <v>32.098999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>67</v>
+      </c>
+      <c r="D11">
+        <v>37.313000000000002</v>
+      </c>
+      <c r="E11">
+        <v>4524</v>
+      </c>
+      <c r="F11">
+        <v>9861</v>
+      </c>
+      <c r="G11">
+        <v>45.878</v>
+      </c>
+      <c r="H11">
+        <v>45.878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>